<commit_message>
Probably many things will be broken - see Obsidian for edits still needed to get things back to working (eventual aim is to be able to have concentrations as input parameters for ISNMFA fitting)
</commit_message>
<xml_diff>
--- a/models/toy/inst_estimation/estimated_concentrations.xlsx
+++ b/models/toy/inst_estimation/estimated_concentrations.xlsx
@@ -445,7 +445,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4.993415330755882</v>
+        <v>4.709842930011267</v>
       </c>
     </row>
     <row r="3">
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.012367784879062</v>
+        <v>0.0840523502246763</v>
       </c>
     </row>
     <row r="4">
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.532899961774737</v>
+        <v>1.084062404365242</v>
       </c>
     </row>
     <row r="5">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1462562446650066</v>
+        <v>0.6827811467223019</v>
       </c>
     </row>
     <row r="6">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.03679199768677659</v>
+        <v>1.461752845699677</v>
       </c>
     </row>
     <row r="7">
@@ -495,7 +495,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.0005295807794183525</v>
+        <v>0.2174853294999878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>